<commit_message>
Refactor the classes to put them into more of a MVC layout. with model being broken up into the separate parts.
</commit_message>
<xml_diff>
--- a/Scrum Sheet.xlsx
+++ b/Scrum Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinnyvalente/Desktop/SCCC/Spring 2020/CSE248 /"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexander\Desktop\College Work\CSE248\CSE248GroupProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B554220-9394-454D-A8BF-3C6CD5DD3669}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4855FB7C-4D30-40C1-8CA8-8F3B4E8CE1E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14660" yWindow="460" windowWidth="13760" windowHeight="16380" xr2:uid="{1519A6EF-D465-BE48-BCF1-CBE758F2DBA9}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1519A6EF-D465-BE48-BCF1-CBE758F2DBA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
   <si>
     <t>Class</t>
   </si>
@@ -80,15 +80,6 @@
     <t>Account Info</t>
   </si>
   <si>
-    <t>2 points</t>
-  </si>
-  <si>
-    <t>1 poiont</t>
-  </si>
-  <si>
-    <t>5 points</t>
-  </si>
-  <si>
     <t>Person on Task</t>
   </si>
   <si>
@@ -107,18 +98,6 @@
     <t>null</t>
   </si>
   <si>
-    <t>vinny</t>
-  </si>
-  <si>
-    <t>jon</t>
-  </si>
-  <si>
-    <t>login</t>
-  </si>
-  <si>
-    <t>alex</t>
-  </si>
-  <si>
     <t>PANE</t>
   </si>
   <si>
@@ -144,12 +123,33 @@
   </si>
   <si>
     <t>Order/ Date and Time</t>
+  </si>
+  <si>
+    <t>Vinny</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Reset Password/Forgot Email</t>
+  </si>
+  <si>
+    <t>1 Point</t>
+  </si>
+  <si>
+    <t>2 Points</t>
+  </si>
+  <si>
+    <t>5 Points</t>
+  </si>
+  <si>
+    <t>Jon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="3">
     <font>
       <sz val="12"/>
@@ -201,8 +201,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{8DB9C4EC-1451-4876-8201-CC024B460D36}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -511,23 +539,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7172CB-218E-634F-8C4E-F928855B0C14}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="23.1640625" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26">
+    <row r="1" spans="1:7" ht="26.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,10 +573,10 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -567,10 +596,10 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -590,15 +619,15 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -613,15 +642,15 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -636,10 +665,10 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -659,10 +688,10 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -681,8 +710,11 @@
       <c r="E7">
         <v>9</v>
       </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -702,10 +734,10 @@
         <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -725,7 +757,7 @@
         <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -745,15 +777,15 @@
         <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="G10" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -768,10 +800,10 @@
         <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -791,10 +823,10 @@
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -814,10 +846,10 @@
         <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -837,60 +869,88 @@
         <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="G14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16">
         <f>E2+E3+E4+E5+E6+E7+E8+E9+E10+E11+E12+E13+E14</f>
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
+        <v>32</v>
+      </c>
+      <c r="F20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished database and filehelper, also updated scrum sheet
</commit_message>
<xml_diff>
--- a/Scrum Sheet.xlsx
+++ b/Scrum Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexander\Desktop\College Work\CSE248\CSE248GroupProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinnyvalente/Desktop/SCCC/Spring 2020/CSE248 /CSE248GroupProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4855FB7C-4D30-40C1-8CA8-8F3B4E8CE1E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27DC09D-1230-AC4A-9C40-36BC45F58B54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1519A6EF-D465-BE48-BCF1-CBE758F2DBA9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16320" xr2:uid="{1519A6EF-D465-BE48-BCF1-CBE758F2DBA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
   <si>
     <t>Class</t>
   </si>
@@ -98,9 +98,6 @@
     <t>null</t>
   </si>
   <si>
-    <t>PANE</t>
-  </si>
-  <si>
     <t>home</t>
   </si>
   <si>
@@ -144,6 +141,15 @@
   </si>
   <si>
     <t>Jon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database / financials </t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>PANE (5pnts EACH PANE)</t>
   </si>
 </sst>
 </file>
@@ -539,24 +545,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7172CB-218E-634F-8C4E-F928855B0C14}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25">
+    <row r="1" spans="1:7" ht="26">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -627,7 +633,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -650,7 +656,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -665,7 +671,7 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
         <v>18</v>
@@ -688,10 +694,10 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -734,10 +740,10 @@
         <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -756,8 +762,11 @@
       <c r="E9">
         <v>4</v>
       </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
       <c r="G9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -785,7 +794,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -800,10 +809,10 @@
         <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -823,10 +832,10 @@
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -846,7 +855,7 @@
         <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G13" t="s">
         <v>18</v>
@@ -869,88 +878,135 @@
         <v>15</v>
       </c>
       <c r="F14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
         <v>36</v>
       </c>
-      <c r="G14" t="s">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>17</v>
+      </c>
+      <c r="F15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="B16" t="s">
+    <row r="19" spans="1:7">
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
         <v>33</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D19" t="s">
         <v>34</v>
       </c>
-      <c r="D16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16">
-        <f>E2+E3+E4+E5+E6+E7+E8+E9+E10+E11+E12+E13+E14</f>
-        <v>116</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" t="s">
+      <c r="E19">
+        <f>E2+E3+E4+E5+E6+E7+E8+E9+E10+E11+E12+E13+E14+E15</f>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28">
+        <v>5</v>
+      </c>
+      <c r="F28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
+      <c r="F29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30">
+        <v>5</v>
+      </c>
+      <c r="F30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" t="s">
+      <c r="E31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
+      <c r="E33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
+      <c r="E34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>26</v>
+      <c r="E35">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Split Database class into order, invoice, product, and user databases
</commit_message>
<xml_diff>
--- a/Scrum Sheet.xlsx
+++ b/Scrum Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinnyvalente/Desktop/SCCC/Spring 2020/CSE248 /CSE248GroupProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27DC09D-1230-AC4A-9C40-36BC45F58B54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDCD0D9-5A74-4B4F-A1E2-91DCBF9200BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16320" xr2:uid="{1519A6EF-D465-BE48-BCF1-CBE758F2DBA9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="39">
   <si>
     <t>Class</t>
   </si>
@@ -146,10 +146,10 @@
     <t xml:space="preserve">Database / financials </t>
   </si>
   <si>
-    <t>done</t>
-  </si>
-  <si>
     <t>PANE (5pnts EACH PANE)</t>
+  </si>
+  <si>
+    <t>jon</t>
   </si>
 </sst>
 </file>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7172CB-218E-634F-8C4E-F928855B0C14}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -766,7 +766,7 @@
         <v>29</v>
       </c>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -924,7 +924,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -966,7 +966,7 @@
         <v>16</v>
       </c>
       <c r="G30" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -976,6 +976,12 @@
       <c r="E31">
         <v>10</v>
       </c>
+      <c r="F31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G31" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
@@ -984,24 +990,42 @@
       <c r="E32">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" t="s">
+        <v>38</v>
+      </c>
+      <c r="G32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>22</v>
       </c>
       <c r="E33">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>24</v>
       </c>
       <c r="E34">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" t="s">
+        <v>29</v>
+      </c>
+      <c r="G34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Fixed dates in Scrum Sheet
</commit_message>
<xml_diff>
--- a/Scrum Sheet.xlsx
+++ b/Scrum Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinnyvalente/Desktop/SCCC/Spring 2020/CSE248 /CSE248GroupProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AEF1C1-2AD7-D342-9336-1D37D08DA13F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC73D454-F5BD-8B40-A41D-669EFE1396D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16380" xr2:uid="{1519A6EF-D465-BE48-BCF1-CBE758F2DBA9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="62">
   <si>
     <t>Weight</t>
   </si>
@@ -219,9 +219,6 @@
   </si>
   <si>
     <t>Class/Assignment</t>
-  </si>
-  <si>
-    <t>2/</t>
   </si>
 </sst>
 </file>
@@ -417,9 +414,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -427,6 +421,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1038,7 +1035,7 @@
   <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="119" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1101,8 +1098,8 @@
       <c r="G2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>62</v>
+      <c r="H2" s="15">
+        <v>43881</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1127,8 +1124,8 @@
       <c r="G3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>62</v>
+      <c r="H3" s="14">
+        <v>43876</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1153,8 +1150,8 @@
       <c r="G4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>62</v>
+      <c r="H4" s="14">
+        <v>43876</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1179,7 +1176,7 @@
       <c r="G5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="14">
         <v>43876</v>
       </c>
     </row>
@@ -1205,7 +1202,7 @@
       <c r="G6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="14">
         <v>43876</v>
       </c>
     </row>
@@ -1231,7 +1228,7 @@
       <c r="G7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="14">
         <v>43882</v>
       </c>
     </row>
@@ -1257,7 +1254,7 @@
       <c r="G8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="14">
         <v>43882</v>
       </c>
     </row>
@@ -1283,7 +1280,7 @@
       <c r="G9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="14">
         <v>43883</v>
       </c>
     </row>
@@ -1309,7 +1306,7 @@
       <c r="G10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="14">
         <v>43882</v>
       </c>
     </row>
@@ -1335,7 +1332,7 @@
       <c r="G11" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="14">
         <v>43883</v>
       </c>
     </row>
@@ -1361,7 +1358,7 @@
       <c r="G12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="14">
         <v>43883</v>
       </c>
     </row>
@@ -1387,7 +1384,7 @@
       <c r="G13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="14">
         <v>43883</v>
       </c>
     </row>
@@ -1413,7 +1410,7 @@
       <c r="G14" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="14">
         <v>43884</v>
       </c>
     </row>
@@ -1439,7 +1436,7 @@
       <c r="G15" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="14">
         <v>43882</v>
       </c>
     </row>
@@ -1476,7 +1473,7 @@
       <c r="G17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H17" s="15">
+      <c r="H17" s="14">
         <v>43876</v>
       </c>
     </row>
@@ -1503,7 +1500,7 @@
       <c r="G18" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18" s="14">
         <v>43883</v>
       </c>
     </row>
@@ -1530,7 +1527,7 @@
       <c r="G19" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H19" s="14">
         <v>43882</v>
       </c>
     </row>
@@ -1557,7 +1554,7 @@
       <c r="G20" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="15">
+      <c r="H20" s="14">
         <v>43877</v>
       </c>
     </row>
@@ -1584,7 +1581,7 @@
       <c r="G21" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21" s="14">
         <v>43877</v>
       </c>
     </row>
@@ -1611,7 +1608,7 @@
       <c r="G22" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="15">
+      <c r="H22" s="14">
         <v>43876</v>
       </c>
     </row>
@@ -1638,7 +1635,7 @@
       <c r="G23" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H23" s="15">
+      <c r="H23" s="14">
         <v>43882</v>
       </c>
     </row>
@@ -1665,7 +1662,7 @@
       <c r="G24" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="15">
+      <c r="H24" s="14">
         <v>43875</v>
       </c>
     </row>
@@ -1692,7 +1689,7 @@
       <c r="G25" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H25" s="15">
+      <c r="H25" s="14">
         <v>43877</v>
       </c>
     </row>
@@ -1719,7 +1716,7 @@
       <c r="G26" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H26" s="15">
+      <c r="H26" s="14">
         <v>43881</v>
       </c>
     </row>
@@ -1746,7 +1743,7 @@
       <c r="G27" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H27" s="15">
+      <c r="H27" s="14">
         <v>43881</v>
       </c>
     </row>
@@ -1773,7 +1770,7 @@
       <c r="G28" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H28" s="15">
+      <c r="H28" s="14">
         <v>43881</v>
       </c>
     </row>
@@ -1800,7 +1797,7 @@
       <c r="G29" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H29" s="15">
+      <c r="H29" s="14">
         <v>43881</v>
       </c>
     </row>
@@ -1827,7 +1824,7 @@
       <c r="G30" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H30" s="15">
+      <c r="H30" s="14">
         <v>43882</v>
       </c>
     </row>
@@ -1854,7 +1851,7 @@
       <c r="G31" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H31" s="15">
+      <c r="H31" s="14">
         <v>43876</v>
       </c>
     </row>
@@ -1881,7 +1878,7 @@
       <c r="G32" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H32" s="15">
+      <c r="H32" s="14">
         <v>43876</v>
       </c>
     </row>
@@ -1908,7 +1905,7 @@
       <c r="G33" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H33" s="15">
+      <c r="H33" s="14">
         <v>43876</v>
       </c>
     </row>
@@ -1935,7 +1932,7 @@
       <c r="G34" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H34" s="15">
+      <c r="H34" s="14">
         <v>43880</v>
       </c>
     </row>
@@ -1962,7 +1959,7 @@
       <c r="G35" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H35" s="15">
+      <c r="H35" s="14">
         <v>43882</v>
       </c>
     </row>
@@ -1989,7 +1986,7 @@
       <c r="G36" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H36" s="15">
+      <c r="H36" s="14">
         <v>43881</v>
       </c>
     </row>
@@ -2016,7 +2013,7 @@
       <c r="G37" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H37" s="15">
+      <c r="H37" s="14">
         <v>43877</v>
       </c>
     </row>
@@ -2043,7 +2040,7 @@
       <c r="G38" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H38" s="15">
+      <c r="H38" s="14">
         <v>43882</v>
       </c>
     </row>
@@ -2070,7 +2067,7 @@
       <c r="G39" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H39" s="15">
+      <c r="H39" s="14">
         <v>43882</v>
       </c>
     </row>
@@ -2097,7 +2094,7 @@
       <c r="G40" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H40" s="15">
+      <c r="H40" s="14">
         <v>43882</v>
       </c>
     </row>
@@ -2124,7 +2121,7 @@
       <c r="G41" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H41" s="15">
+      <c r="H41" s="14">
         <v>43881</v>
       </c>
     </row>
@@ -2151,7 +2148,7 @@
       <c r="G42" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H42" s="15">
+      <c r="H42" s="14">
         <v>43881</v>
       </c>
     </row>
@@ -2178,7 +2175,7 @@
       <c r="G43" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H43" s="15">
+      <c r="H43" s="14">
         <v>43882</v>
       </c>
     </row>
@@ -2205,7 +2202,7 @@
       <c r="G44" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H44" s="15">
+      <c r="H44" s="14">
         <v>43877</v>
       </c>
     </row>
@@ -2217,7 +2214,7 @@
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
       <c r="G45" s="8"/>
-      <c r="H45" s="15"/>
+      <c r="H45" s="14"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="6" t="s">
@@ -2241,7 +2238,7 @@
       <c r="G46" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H46" s="15">
+      <c r="H46" s="14">
         <v>43874</v>
       </c>
     </row>
@@ -2267,7 +2264,7 @@
       <c r="G47" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H47" s="15">
+      <c r="H47" s="14">
         <v>43874</v>
       </c>
     </row>
@@ -2293,7 +2290,7 @@
       <c r="G48" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H48" s="15">
+      <c r="H48" s="14">
         <v>43884</v>
       </c>
     </row>
@@ -2314,52 +2311,52 @@
       <c r="D50" s="11"/>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
-      <c r="G50" s="14"/>
+      <c r="G50" s="13"/>
       <c r="H50" s="11"/>
     </row>
     <row r="51" spans="1:8">
-      <c r="D51" s="13" t="s">
+      <c r="D51" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E51" s="13">
+      <c r="E51" s="12">
         <f>E44+E43+E42+E41+E40+E39+E38+E37+E36+E35+E34+E33+E32+E31+E30+E29+E28+E27+E26+E25+E24+E23+E22+E21+E20+E19+E18+E17+E10+E9+E8+E7+E6+E5+E4+E3+E2+E46+E47+E48+E49</f>
         <v>563</v>
       </c>
-      <c r="F51" s="13"/>
+      <c r="F51" s="12"/>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="13"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
     </row>
     <row r="53" spans="1:8">
-      <c r="D53" s="13"/>
-      <c r="E53" s="13">
+      <c r="D53" s="12"/>
+      <c r="E53" s="12">
         <f>COUNTIF($F$2:$F$50,"Alex")</f>
         <v>18</v>
       </c>
-      <c r="F53" s="13" t="s">
+      <c r="F53" s="12" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="D54" s="13"/>
-      <c r="E54" s="13">
+      <c r="D54" s="12"/>
+      <c r="E54" s="12">
         <f>COUNTIF($F$2:$F$50,"Vinny")</f>
         <v>19</v>
       </c>
-      <c r="F54" s="13" t="s">
+      <c r="F54" s="12" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="D55" s="13"/>
-      <c r="E55" s="13">
+      <c r="D55" s="12"/>
+      <c r="E55" s="12">
         <f>COUNTIF($F$2:$F$50,"Jon")</f>
         <v>8</v>
       </c>
-      <c r="F55" s="13" t="s">
+      <c r="F55" s="12" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>